<commit_message>
Fixed trafo model to be good enough
</commit_message>
<xml_diff>
--- a/simplepower/models/grid_data5.xlsx
+++ b/simplepower/models/grid_data5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uisn-my.sharepoint.com/personal/emelf_usn_no/Documents/PhD - SysOpt/Python Work/Custom Modules/simplepower/simplepower/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E82FE53-CFA4-4BCC-A63C-7261D658D8EE}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DBC9EC7-16D5-4C1B-86E0-08FF5197C43F}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{120A7045-FD09-44EC-B7BA-2F1FCE4B68C8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{120A7045-FD09-44EC-B7BA-2F1FCE4B68C8}"/>
   </bookViews>
   <sheets>
     <sheet name="busbars" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F24F74-C913-4254-AF10-9102B3F26C94}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92C15A9-E0D3-48E6-90F6-6A9120B37C7B}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,10 +798,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="I2">
         <v>0</v>

</xml_diff>